<commit_message>
fix: remove Imagination categories
</commit_message>
<xml_diff>
--- a/Data/1800-1839_metadata.xlsx
+++ b/Data/1800-1839_metadata.xlsx
@@ -5953,11 +5953,7 @@
       <c r="T65" t="n">
         <v>20221209</v>
       </c>
-      <c r="U65" t="inlineStr">
-        <is>
-          <t>Diktning: Lyrikk</t>
-        </is>
-      </c>
+      <c r="U65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -6552,11 +6548,7 @@
       <c r="T72" t="n">
         <v>20221209</v>
       </c>
-      <c r="U72" t="inlineStr">
-        <is>
-          <t>Diktning: Lyrikk</t>
-        </is>
-      </c>
+      <c r="U72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -8904,11 +8896,7 @@
       <c r="T100" t="n">
         <v>20221209</v>
       </c>
-      <c r="U100" t="inlineStr">
-        <is>
-          <t>Diktning: Lyrikk</t>
-        </is>
-      </c>
+      <c r="U100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">

</xml_diff>